<commit_message>
Fix Spacing in Screen Shots
</commit_message>
<xml_diff>
--- a/assets/testing.xlsx
+++ b/assets/testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jane\OneDrive\3. EDUCATION\FULLSTACK SOFTWARE DEVELOPMENT DIPLOMA\MS-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDC5EAC-B415-415D-9224-A2D0AC9E267F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B85F4E3-772A-4ED3-B6A5-27FD274557C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19280" yWindow="-80" windowWidth="19360" windowHeight="10360" activeTab="2" xr2:uid="{5A23EB50-F6EE-45F3-A5F7-94914E52C60F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5A23EB50-F6EE-45F3-A5F7-94914E52C60F}"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
   <si>
     <t>Wild Thing Yoga Test Criteria</t>
   </si>
@@ -374,6 +374,30 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -391,42 +415,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -750,13 +750,13 @@
   <dimension ref="B1:O11"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="29.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="2.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="29" style="2" customWidth="1"/>
     <col min="5" max="6" width="27.42578125" style="2" customWidth="1"/>
@@ -766,14 +766,14 @@
   <sheetData>
     <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" s="4" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -788,122 +788,124 @@
         <v>24</v>
       </c>
       <c r="C3" s="6"/>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="28"/>
       <c r="G3" s="7" t="s">
         <v>2</v>
       </c>
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="2:15" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="12"/>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
       <c r="G4" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="107.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="15" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="12"/>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
       <c r="G5" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="15" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="12"/>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="14"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="14" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="2:15" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="15" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="12"/>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
       <c r="G7" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="80.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="16" t="s">
         <v>33</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
       <c r="G8" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="16" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="9"/>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
       <c r="G9" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:15" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="16" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="9"/>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
       <c r="G10" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="2:15" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="16" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="9"/>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
       <c r="G11" s="10" t="s">
         <v>6</v>
       </c>
@@ -947,14 +949,14 @@
   <sheetData>
     <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" s="4" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -969,11 +971,11 @@
         <v>15</v>
       </c>
       <c r="C3" s="6"/>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="28"/>
       <c r="G3" s="7" t="s">
         <v>2</v>
       </c>
@@ -984,11 +986,11 @@
         <v>16</v>
       </c>
       <c r="C4" s="12"/>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
       <c r="G4" s="13" t="s">
         <v>6</v>
       </c>
@@ -998,11 +1000,11 @@
         <v>17</v>
       </c>
       <c r="C5" s="12"/>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="13" t="s">
         <v>6</v>
       </c>
@@ -1012,11 +1014,11 @@
         <v>18</v>
       </c>
       <c r="C6" s="12"/>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
       <c r="G6" s="13" t="s">
         <v>6</v>
       </c>
@@ -1026,11 +1028,11 @@
         <v>20</v>
       </c>
       <c r="C7" s="12"/>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
       <c r="G7" s="13" t="s">
         <v>6</v>
       </c>
@@ -1056,7 +1058,7 @@
   <dimension ref="B1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,14 +1074,14 @@
   <sheetData>
     <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" s="4" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -1094,137 +1096,139 @@
         <v>3</v>
       </c>
       <c r="C3" s="6"/>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="28"/>
       <c r="G3" s="7" t="s">
         <v>2</v>
       </c>
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="2:15" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="24" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="28" t="s">
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="19" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="24" t="s">
+      <c r="C5" s="18"/>
+      <c r="D5" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="28" t="s">
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="19" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="29" t="s">
+      <c r="C6" s="18"/>
+      <c r="D6" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="28" t="s">
+      <c r="E6" s="29"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="19" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="24" t="s">
+      <c r="C7" s="18"/>
+      <c r="D7" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="26" t="s">
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="24" t="s">
+      <c r="C8" s="18"/>
+      <c r="D8" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="26" t="s">
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="29" t="s">
+      <c r="C9" s="18"/>
+      <c r="D9" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="28"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="19" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="2:15" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="24" t="s">
+      <c r="C10" s="18"/>
+      <c r="D10" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="31" t="s">
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="20" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="2:15" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="24" t="s">
+      <c r="C11" s="18"/>
+      <c r="D11" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="31" t="s">
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="20" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="24" t="s">
+      <c r="C12" s="18"/>
+      <c r="D12" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="31" t="s">
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="20" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>